<commit_message>
Ciclo 3 terminado, lab enviado
</commit_message>
<xml_diff>
--- a/Laboratorio 2/Tabla Ciclos.xlsx
+++ b/Laboratorio 2/Tabla Ciclos.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="64">
   <si>
     <t>Ciclo</t>
   </si>
@@ -180,6 +180,42 @@
   </si>
   <si>
     <t>deberiaCrearUnaMatrizAPartirDeMatrizDeFraccionarios</t>
+  </si>
+  <si>
+    <t>multiplique</t>
+  </si>
+  <si>
+    <t>productoMatricial</t>
+  </si>
+  <si>
+    <t>deberiaMultiplicarFraccionariosCorrectamente</t>
+  </si>
+  <si>
+    <t>laMultiplicacionDeberiaFuncionarConCero</t>
+  </si>
+  <si>
+    <t>laMultiplicacionDeberiaFuncionarConNegativos</t>
+  </si>
+  <si>
+    <t>laMultiplicacionDeberiaSerConmutativa</t>
+  </si>
+  <si>
+    <t>multipliqueDeberiaFuncionarParaMatricesDelMismoTamaño</t>
+  </si>
+  <si>
+    <t>ProdMatricialDeberiaFuncionarParaMatricesCompatibles</t>
+  </si>
+  <si>
+    <t>ProdMatricialDeberiaRetornarNuloSiSonDeDiferenteTamaño</t>
+  </si>
+  <si>
+    <t>hacerUnaMultiplicacionNoDeberiaAlterarLasMatricesOriginales</t>
+  </si>
+  <si>
+    <t>hacerUnProductoMatricialNoDeberiaAlterarLasMatricesOriginales</t>
+  </si>
+  <si>
+    <t>multipliqueDeberiaRetornarNuloSiSonDeDiferenteTamaño</t>
   </si>
 </sst>
 </file>
@@ -486,34 +522,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -796,10 +832,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H20"/>
+  <dimension ref="B1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -807,11 +843,11 @@
     <col min="1" max="1" width="4.42578125" style="2" customWidth="1"/>
     <col min="2" max="2" width="5.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="52" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="56.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="60.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="57.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="67.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="66.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
@@ -840,7 +876,7 @@
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="9">
+      <c r="B3" s="16">
         <v>1</v>
       </c>
       <c r="C3" s="7" t="s">
@@ -858,12 +894,12 @@
       <c r="G3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="9" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="11"/>
+      <c r="B4" s="17"/>
       <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
@@ -879,12 +915,12 @@
       <c r="G4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="12" t="s">
+      <c r="H4" s="10" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="11"/>
+      <c r="B5" s="17"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
@@ -896,12 +932,12 @@
       <c r="G5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="H5" s="10" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="11"/>
+      <c r="B6" s="17"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
@@ -913,101 +949,101 @@
       <c r="G6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="12" t="s">
+      <c r="H6" s="10" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="11"/>
+      <c r="B7" s="17"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
-      <c r="H7" s="12" t="s">
+      <c r="H7" s="10" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="11"/>
+      <c r="B8" s="17"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
-      <c r="H8" s="12" t="s">
+      <c r="H8" s="10" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="11"/>
+      <c r="B9" s="17"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="12" t="s">
+      <c r="H9" s="10" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="11"/>
+      <c r="B10" s="17"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
-      <c r="H10" s="12" t="s">
+      <c r="H10" s="10" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="11"/>
+      <c r="B11" s="17"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
-      <c r="H11" s="12" t="s">
+      <c r="H11" s="10" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="12" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="11"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="18" t="s">
+      <c r="B12" s="17"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="15" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="9">
+      <c r="B13" s="16">
         <v>2</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="D13" s="12" t="s">
         <v>47</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F13" s="16" t="s">
+      <c r="F13" s="13" t="s">
         <v>51</v>
       </c>
       <c r="G13" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="H13" s="10" t="s">
+      <c r="H13" s="9" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="11"/>
+      <c r="B14" s="17"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1" t="s">
         <v>48</v>
@@ -1021,12 +1057,12 @@
       <c r="G14" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H14" s="12" t="s">
+      <c r="H14" s="10" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="11"/>
+      <c r="B15" s="17"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1" t="s">
         <v>49</v>
@@ -1038,12 +1074,12 @@
         <v>43</v>
       </c>
       <c r="G15" s="1"/>
-      <c r="H15" s="12" t="s">
+      <c r="H15" s="10" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="11"/>
+      <c r="B16" s="17"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1" t="s">
         <v>50</v>
@@ -1055,12 +1091,12 @@
         <v>44</v>
       </c>
       <c r="G16" s="1"/>
-      <c r="H16" s="12" t="s">
+      <c r="H16" s="10" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="11"/>
+      <c r="B17" s="17"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -1068,12 +1104,12 @@
         <v>45</v>
       </c>
       <c r="G17" s="1"/>
-      <c r="H17" s="12" t="s">
+      <c r="H17" s="10" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="11"/>
+      <c r="B18" s="17"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -1081,34 +1117,92 @@
         <v>46</v>
       </c>
       <c r="G18" s="1"/>
-      <c r="H18" s="12" t="s">
+      <c r="H18" s="10" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="19" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="13"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="14" t="s">
+      <c r="B19" s="17"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="15" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
+      <c r="B20" s="16">
+        <v>3</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="17"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G21" s="1"/>
+      <c r="H21" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="17"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G22" s="1"/>
+      <c r="H22" s="10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="18"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G23" s="8"/>
+      <c r="H23" s="11" t="s">
+        <v>57</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B3:B12"/>
     <mergeCell ref="B13:B19"/>
+    <mergeCell ref="B20:B23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>